<commit_message>
calibration curves with manual rock movements are DONEEEEEEEEEEEEEEEEEE
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/ManualRockMovements-2/mov2_calibration_curve.xlsx
+++ b/Hydrophones/Calibration/ManualRockMovements-2/mov2_calibration_curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Calibration\ManualRockMovements-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED23D56-DE92-4195-B300-8A7EF8F92BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D61B9AD-A0CD-4FEB-98A8-89C3C7CBBECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,21 +46,6 @@
   </si>
   <si>
     <t>Env Max A</t>
-  </si>
-  <si>
-    <t>Aprox Time Start</t>
-  </si>
-  <si>
-    <t>Aprox Time End</t>
-  </si>
-  <si>
-    <t>interspace</t>
-  </si>
-  <si>
-    <t>duration (s)</t>
-  </si>
-  <si>
-    <t>avg</t>
   </si>
   <si>
     <t>id</t>
@@ -118,6 +103,21 @@
   </si>
   <si>
     <t>in seconds</t>
+  </si>
+  <si>
+    <t>Total Max A</t>
+  </si>
+  <si>
+    <t>Start (s)</t>
+  </si>
+  <si>
+    <t>End (s)</t>
+  </si>
+  <si>
+    <t>Dmax</t>
+  </si>
+  <si>
+    <t>Total Dmax</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,13 +237,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,7 +323,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs Particle Size</a:t>
+              <a:t> vs Dmax</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -345,7 +368,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -418,94 +441,91 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$26</c:f>
+              <c:f>Sheet1!$G$2:$G$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
                 <c:pt idx="4">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>45</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>45</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>64</c:v>
+                <c:pt idx="21">
+                  <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>64</c:v>
+                <c:pt idx="25">
+                  <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>45</c:v>
+                <c:pt idx="29">
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$25</c:f>
+              <c:f>Sheet1!$F$2:$F$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>2.8199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.2899999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1047</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.3900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.32800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.18690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.22800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.29139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.1199999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.21579999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -569,7 +589,513 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Diameter</a:t>
+                  <a:t>Dmax</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299627312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="299627312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Max Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299639312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Amax</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Total Dmax</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.28995050618672669"/>
+                  <c:y val="8.0404040404040408E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>6.2899999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1047</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.32800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.29139999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-19B5-4C91-8B55-BB3D3B434336}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="299639312"/>
+        <c:axId val="299627312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="299639312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Dmax</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
@@ -858,6 +1384,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1374,20 +1940,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1407,6 +2489,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>676276</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D8B3ABD-EDC9-4460-B639-A9792CBB4407}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1678,742 +2798,831 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="18.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
+      <c r="B2" s="16">
+        <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="5">
         <v>32</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="H2" s="1">
-        <f>E2-D2</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <f t="shared" ref="I2:I24" si="0">D3-E2</f>
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2">
-        <f>AVERAGE(I2:I24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="19">
+        <v>50</v>
+      </c>
+      <c r="E2" s="19">
+        <v>70</v>
+      </c>
+      <c r="F2" s="19">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="G2" s="19">
+        <f>MAX(C2:C3)</f>
+        <v>32</v>
+      </c>
+      <c r="H2" s="19">
+        <f>MAX(F2:F7)</f>
+        <v>6.2899999999999998E-2</v>
+      </c>
+      <c r="I2" s="19">
+        <f>MAX(G2:G7)</f>
+        <v>32</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="9">
         <v>32</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3:H25" si="1">E3-D3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <f t="shared" ref="A4:A34" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>32</v>
+      </c>
+      <c r="D4" s="20">
+        <v>70</v>
+      </c>
+      <c r="E4" s="20">
+        <v>90</v>
+      </c>
+      <c r="F4" s="20">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="G4" s="20">
+        <f>MAX(C4:C5)</f>
+        <v>32</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <f t="shared" ref="A4:A34" si="2">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="C5" s="9">
         <v>32</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="H4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>1</v>
+      <c r="B6" s="17">
+        <v>1.3</v>
       </c>
       <c r="C6" s="7">
         <v>32</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="H6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="D6" s="20">
+        <v>90</v>
+      </c>
+      <c r="E6" s="20">
+        <v>100</v>
+      </c>
+      <c r="F6" s="20">
+        <v>6.2899999999999998E-2</v>
+      </c>
+      <c r="G6" s="20">
+        <f>MAX(C6:C7)</f>
+        <v>32</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B7" s="8">
-        <v>1</v>
+      <c r="B7" s="18">
+        <v>1.3</v>
       </c>
       <c r="C7" s="9">
         <v>32</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="H7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B8" s="4">
-        <v>2</v>
+      <c r="B8" s="16">
+        <v>2.1</v>
       </c>
       <c r="C8" s="5">
         <v>32</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="H8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="D8" s="19">
+        <v>120</v>
+      </c>
+      <c r="E8" s="19">
+        <v>140</v>
+      </c>
+      <c r="F8" s="19">
+        <v>9.8299999999999998E-2</v>
+      </c>
+      <c r="G8" s="19">
+        <f>MAX(C8:C9)</f>
+        <v>45</v>
+      </c>
+      <c r="H8" s="19">
+        <f>MAX(F8:F13)</f>
+        <v>0.1047</v>
+      </c>
+      <c r="I8" s="19">
+        <f>MAX(G8:G13)</f>
+        <v>45</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="17">
+        <v>2.1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>45</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C10" s="5">
         <v>32</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="D10" s="20">
+        <v>140</v>
+      </c>
+      <c r="E10" s="20">
+        <v>155</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0.1047</v>
+      </c>
+      <c r="G10" s="20">
+        <f>MAX(C10:C11)</f>
+        <v>45</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="6">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C11" s="11">
+        <v>45</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C12" s="7">
         <v>32</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="H10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="D12" s="20">
+        <v>160</v>
+      </c>
+      <c r="E12" s="20">
+        <v>170</v>
+      </c>
+      <c r="F12" s="20">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="G12" s="20">
+        <f>MAX(C12:C13)</f>
+        <v>45</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>2</v>
-      </c>
-      <c r="C11" s="10">
-        <v>45</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="H11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <v>2</v>
-      </c>
-      <c r="C12" s="10">
-        <v>45</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="H12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B13" s="8">
-        <v>2</v>
+      <c r="B13" s="18">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C13" s="11">
         <v>45</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="H13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B14" s="4">
-        <v>3</v>
+      <c r="B14" s="16">
+        <v>3.1</v>
       </c>
       <c r="C14" s="5">
         <v>32</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="H14" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="D14" s="19">
+        <v>190</v>
+      </c>
+      <c r="E14" s="19">
+        <v>210</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="G14" s="19">
+        <f>MAX(C14:C16)</f>
+        <v>64</v>
+      </c>
+      <c r="H14" s="19">
+        <f>MAX(F14:F22)</f>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="I14" s="19">
+        <f>MAX(G14:G22)</f>
+        <v>64</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B15" s="6">
-        <v>3</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="B15" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="C15" s="10">
+        <v>45</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="C16" s="13">
+        <v>64</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="17">
+        <v>3.2</v>
+      </c>
+      <c r="C17" s="5">
         <v>32</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="D17" s="23">
+        <v>215</v>
+      </c>
+      <c r="E17" s="23">
+        <v>230</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0.18690000000000001</v>
+      </c>
+      <c r="G17" s="23">
+        <f>MAX(C17:C19)</f>
+        <v>64</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="6">
-        <v>3</v>
-      </c>
-      <c r="C16" s="7">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="H16" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="6">
-        <v>3</v>
-      </c>
-      <c r="C17" s="10">
-        <v>45</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="H17" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="B18" s="6">
-        <v>3</v>
+      <c r="B18" s="17">
+        <v>3.2</v>
       </c>
       <c r="C18" s="10">
         <v>45</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="H18" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B19" s="6">
-        <v>3</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="B19" s="17">
+        <v>3.2</v>
+      </c>
+      <c r="C19" s="13">
+        <v>64</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="C20" s="7">
+        <v>32</v>
+      </c>
+      <c r="D20" s="20">
+        <v>230</v>
+      </c>
+      <c r="E20" s="20">
+        <v>250</v>
+      </c>
+      <c r="F20" s="20">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="G20" s="20">
+        <f>MAX(C20:C22)</f>
+        <v>64</v>
+      </c>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="C21" s="10">
         <v>45</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="H19" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="6">
-        <v>3</v>
-      </c>
-      <c r="C20" s="12">
-        <v>64</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="H20" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="6">
-        <v>3</v>
-      </c>
-      <c r="C21" s="12">
-        <v>64</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="H21" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="B22" s="8">
-        <v>3</v>
+      <c r="B22" s="18">
+        <v>3.3</v>
       </c>
       <c r="C22" s="13">
         <v>64</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="H22" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="B23" s="4">
-        <v>4</v>
+      <c r="B23" s="16">
+        <v>4.0999999999999996</v>
       </c>
       <c r="C23" s="5">
         <v>32</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="H23" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="D23" s="19">
+        <v>270</v>
+      </c>
+      <c r="E23" s="19">
+        <v>285</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0.29139999999999999</v>
+      </c>
+      <c r="G23" s="19">
+        <f>MAX(C23:C26)</f>
+        <v>90</v>
+      </c>
+      <c r="H23" s="19">
+        <f>MAX(F23:F34)</f>
+        <v>0.29139999999999999</v>
+      </c>
+      <c r="I23" s="19">
+        <f>MAX(G23:G34)</f>
+        <v>90</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="B24" s="6">
-        <v>4</v>
-      </c>
-      <c r="C24" s="7">
+      <c r="B24" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C24" s="10">
+        <v>45</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C25" s="12">
+        <v>64</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C26" s="15">
+        <v>90</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="17">
+        <v>4.2</v>
+      </c>
+      <c r="C27" s="5">
         <v>32</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="H24" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="D27" s="23">
+        <v>290</v>
+      </c>
+      <c r="E27" s="23">
+        <v>310</v>
+      </c>
+      <c r="F27" s="23">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="G27" s="23">
+        <f>MAX(C27:C30)</f>
+        <v>90</v>
+      </c>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="6">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7">
-        <v>32</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="H25" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="6">
-        <v>4</v>
-      </c>
-      <c r="C26" s="10">
-        <v>45</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="6">
-        <v>4</v>
-      </c>
-      <c r="C27" s="10">
-        <v>45</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="B28" s="6">
-        <v>4</v>
+      <c r="B28" s="17">
+        <v>4.2</v>
       </c>
       <c r="C28" s="10">
         <v>45</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="6">
-        <v>4</v>
+      <c r="B29" s="17">
+        <v>4.2</v>
       </c>
       <c r="C29" s="12">
         <v>64</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="6">
-        <v>4</v>
-      </c>
-      <c r="C30" s="12">
+      <c r="B30" s="17">
+        <v>4.2</v>
+      </c>
+      <c r="C30" s="15">
+        <v>90</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="17">
+        <v>4.3</v>
+      </c>
+      <c r="C31" s="7">
+        <v>32</v>
+      </c>
+      <c r="D31" s="20">
+        <v>310</v>
+      </c>
+      <c r="E31" s="20">
+        <v>330</v>
+      </c>
+      <c r="F31" s="20">
+        <v>0.21579999999999999</v>
+      </c>
+      <c r="G31" s="20">
+        <f>MAX(C31:C34)</f>
+        <v>90</v>
+      </c>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="17">
+        <v>4.3</v>
+      </c>
+      <c r="C32" s="10">
+        <v>45</v>
+      </c>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="17">
+        <v>4.3</v>
+      </c>
+      <c r="C33" s="12">
         <v>64</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="6">
-        <v>4</v>
-      </c>
-      <c r="C31" s="12">
-        <v>64</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="6">
-        <v>4</v>
-      </c>
-      <c r="C32" s="15">
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="18">
+        <v>4.3</v>
+      </c>
+      <c r="C34" s="15">
         <v>90</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="6">
-        <v>4</v>
-      </c>
-      <c r="C33" s="15">
-        <v>90</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="8">
-        <v>4</v>
-      </c>
-      <c r="C34" s="16">
-        <v>90</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="17"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C38" s="2">
         <v>0.60364583333333333</v>
@@ -2421,17 +3630,17 @@
       <c r="D38" s="1">
         <v>0</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C39" s="2">
         <v>0.60420138888888886</v>
@@ -2440,137 +3649,151 @@
         <f>C39-$C$38</f>
         <v>5.5555555555553138E-4</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2"/>
+      <c r="F39" s="3">
         <v>48</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="2">
+      <c r="G39" s="3"/>
+      <c r="I39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="2">
         <f>D40-D39</f>
         <v>7.2916666666666963E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C40" s="2">
         <v>0.60493055555555553</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" ref="D40:D45" si="3">C40-$C$38</f>
+        <f t="shared" ref="D40:D45" si="1">C40-$C$38</f>
         <v>1.284722222222201E-3</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2"/>
+      <c r="F40" s="3">
         <f>51+60</f>
         <v>111</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="2">
+      <c r="G40" s="3"/>
+      <c r="I40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="2">
         <f>D42-D41</f>
         <v>7.5231481481474738E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C41" s="2">
         <v>0.60502314814814817</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.3773148148148451E-3</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2"/>
+      <c r="F41" s="3">
         <f>59+60</f>
         <v>119</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="2">
+      <c r="G41" s="3"/>
+      <c r="I41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" s="2">
         <f>D44-D43</f>
         <v>7.6388888888889728E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C42" s="2">
         <v>0.60577546296296292</v>
       </c>
       <c r="D42" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.1296296296295925E-3</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2"/>
+      <c r="F42" s="3">
         <f>4+60*3</f>
         <v>184</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="2">
+      <c r="G42" s="3"/>
+      <c r="I42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42" s="2">
         <f>D46-D45</f>
         <v>1.0763888888889461E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C43" s="2">
         <v>0.60584490740740737</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.1990740740740478E-3</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2"/>
+      <c r="F43" s="3">
         <f>10+60*3</f>
         <v>190</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C44" s="2">
         <v>0.60660879629629627</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.962962962962945E-3</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2"/>
+      <c r="F44" s="3">
         <f>16+60*4</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C45" s="2">
         <v>0.60657407407407404</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.9282407407407174E-3</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2"/>
+      <c r="F45" s="3">
         <f>13+60*4</f>
         <v>253</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C46" s="2">
         <v>0.60765046296296299</v>
@@ -2579,12 +3802,72 @@
         <f>C46-$C$38</f>
         <v>4.0046296296296635E-3</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2"/>
+      <c r="F46" s="3">
         <f>46+60*5</f>
         <v>346</v>
       </c>
+      <c r="G46" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="56">
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="I14:I22"/>
+    <mergeCell ref="I23:I34"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="H14:H22"/>
+    <mergeCell ref="H23:H34"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2592,10 +3875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1036A414-1109-4572-9B8B-8712D66EE434}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="B2" sqref="B2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,136 +3887,404 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" s="22">
+        <v>50</v>
+      </c>
+      <c r="C2" s="22">
+        <v>70</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="B3" s="22">
+        <v>70</v>
+      </c>
+      <c r="C3" s="22">
+        <v>90</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="B4" s="22">
+        <v>90</v>
+      </c>
+      <c r="C4" s="22">
+        <v>100</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="B5" s="22">
+        <v>120</v>
+      </c>
+      <c r="C5" s="22">
+        <v>140</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B6" s="22">
+        <v>140</v>
+      </c>
+      <c r="C6" s="22">
+        <v>155</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B7" s="22">
+        <v>160</v>
+      </c>
+      <c r="C7" s="22">
+        <v>170</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="B8" s="22">
+        <v>190</v>
+      </c>
+      <c r="C8" s="22">
+        <v>210</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="B9" s="22">
+        <v>215</v>
+      </c>
+      <c r="C9" s="22">
+        <v>230</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="B10" s="22">
+        <v>230</v>
+      </c>
+      <c r="C10" s="22">
+        <v>250</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B11" s="22">
+        <v>270</v>
+      </c>
+      <c r="C11" s="22">
+        <v>285</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="B12" s="22">
+        <v>290</v>
+      </c>
+      <c r="C12" s="22">
+        <v>310</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="B13" s="22">
+        <v>310</v>
+      </c>
+      <c r="C13" s="22">
+        <v>330</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>